<commit_message>
Teaching Lab Four bar is now verified
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/RMSE_Results/E/AngVel/result1_csv/RMSE.xlsx
+++ b/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/RMSE_Results/E/AngVel/result1_csv/RMSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teachinglab\Desktop\PMKS_Verification\Mechanisms\Four_Bar_Mechanism\TeachingLab_Four_Bar\RMSE_Results\E\AngVel\result1_csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E036DA-5796-4829-A740-C68948ADAD61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A863CD4-BE36-485A-A9D4-6384B2858068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7095" yWindow="1770" windowWidth="21600" windowHeight="11295" xr2:uid="{7CDB513D-64D3-4A22-9FD4-00D023FF2D75}"/>
+    <workbookView xWindow="7095" yWindow="1770" windowWidth="21600" windowHeight="11295" xr2:uid="{CD81EC31-928D-447D-B1ED-B3388D8FD097}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18202A2B-CAFA-4A3B-AAF5-444705AFE3FD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{076F0DED-BCAF-4F8B-A5BF-E7C48C4EE380}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>